<commit_message>
Added back Monthly CatA file
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite MonthlyCatA201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite MonthlyCatA201718.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="3564" windowWidth="10152" xWindow="0" yWindow="2376"/>
+    <workbookView activeTab="3" windowHeight="4452" windowWidth="14340" xWindow="384" yWindow="84"/>
   </bookViews>
   <sheets>
     <sheet name="first" r:id="rId1" sheetId="1"/>
@@ -12,13 +12,12 @@
     <sheet name="ProcessPayrollForNIMonthly" r:id="rId3" sheetId="4"/>
     <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:B8"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="51">
   <si>
     <t>TC</t>
   </si>
@@ -573,7 +572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1276,7 +1275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>